<commit_message>
Completed Combining Package Routes
</commit_message>
<xml_diff>
--- a/Data/Excel/nodes.xlsx
+++ b/Data/Excel/nodes.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\spares-together\Data\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\spares-together\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C976D4BA-9ECA-4200-B578-C0AB12785090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D1A039-F2B8-4762-8572-DB5FACE19DB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="2715" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00FFFBBB-EAD6-4E68-AFFA-2FCD1F61FB37}"/>
+    <workbookView xWindow="8610" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{00FFFBBB-EAD6-4E68-AFFA-2FCD1F61FB37}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="connections1" sheetId="2" r:id="rId2"/>
+    <sheet name="connections" sheetId="2" r:id="rId2"/>
     <sheet name="vehicle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="25">
   <si>
     <t>Node</t>
   </si>
@@ -100,6 +100,9 @@
   <si>
     <t>Max_Weight</t>
   </si>
+  <si>
+    <t>SupplyDepot</t>
+  </si>
 </sst>
 </file>
 
@@ -134,9 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -195,8 +201,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{900ACE7B-80E4-460A-920B-4032A2BE0BBE}" name="Table1" displayName="Table1" ref="A1:C17" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:C17" xr:uid="{ECEF3D69-C835-406E-B8F2-2264DEE0C0CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{900ACE7B-80E4-460A-920B-4032A2BE0BBE}" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:C18" xr:uid="{ECEF3D69-C835-406E-B8F2-2264DEE0C0CD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9A0D5FDB-2C7D-4488-928D-ADA6C980C87E}" name="Node" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{DFB058DD-1C8F-480E-B21B-995EBD5200A9}" name="X_Coord" dataDxfId="7">
@@ -211,15 +217,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BA641A52-7AB9-43A7-9514-61488BA355D7}" name="Table2" displayName="Table2" ref="A1:D121" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D121" xr:uid="{04C88447-8391-4A32-9E52-E481DB5B8D84}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BA641A52-7AB9-43A7-9514-61488BA355D7}" name="Table2" displayName="Table2" ref="A1:D137" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D137" xr:uid="{04C88447-8391-4A32-9E52-E481DB5B8D84}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BCD01E8D-45ED-4C0F-8BB5-A300C4A8D388}" name="Node_A" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B3464EB2-C8AA-440B-ADC8-06D485DFF6AA}" name="Node_B" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{48B40400-D6BF-47C1-8717-1F36EDD1586A}" name="Connection" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{48B40400-D6BF-47C1-8717-1F36EDD1586A}" name="Connection" dataDxfId="1">
       <calculatedColumnFormula>IF(RAND() &lt; 0.7, 1, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9620C4F3-1855-4926-B3A0-B6FB5CDFB476}" name="Distance" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{9620C4F3-1855-4926-B3A0-B6FB5CDFB476}" name="Distance" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -524,15 +530,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77B6494-BFFD-4D22-9DBF-110F82DECE7B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="10.28515625" style="1" customWidth="1"/>
@@ -555,163 +561,163 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1">
-        <f t="shared" ref="B2:C17" ca="1" si="0">_xlfn.FLOOR.MATH((RAND()*20))</f>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH((RAND()*20))</f>
         <v>12</v>
       </c>
-      <c r="C2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+      <c r="C2" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH((RAND()*20))</f>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <f t="shared" ref="B3:C18" ca="1" si="0">_xlfn.FLOOR.MATH((RAND()*20))</f>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>13</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -719,46 +725,59 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="B18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -771,13 +790,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5722A094-0CD9-419A-845D-F9766D927A5E}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -795,302 +817,302 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <f t="shared" ref="C2:C33" ca="1" si="0">IF(RAND() &lt; 0.7, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+      <c r="C2" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="C17" s="2">
+        <f ca="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="C18:C49" ca="1" si="0">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
@@ -1099,26 +1121,26 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1126,15 +1148,15 @@
       </c>
       <c r="D22" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1147,26 +1169,26 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1174,15 +1196,15 @@
       </c>
       <c r="D25" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1190,15 +1212,15 @@
       </c>
       <c r="D26" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1206,15 +1228,15 @@
       </c>
       <c r="D27" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1222,47 +1244,47 @@
       </c>
       <c r="D28" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1270,15 +1292,15 @@
       </c>
       <c r="D31" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1286,15 +1308,15 @@
       </c>
       <c r="D32" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1302,35 +1324,35 @@
       </c>
       <c r="D33" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ref="C34:C65" ca="1" si="1">IF(RAND() &lt; 0.7, 1, 0)</f>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
@@ -1339,270 +1361,270 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>14</v>
-      </c>
-      <c r="C36" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>15</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D38" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D39" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="D41" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D42" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="D43" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D44" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D45" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>12</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C47" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="D48" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="D49" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="C50:C81" ca="1" si="1">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>0</v>
       </c>
       <c r="D50" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
@@ -1611,26 +1633,26 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1638,47 +1660,47 @@
       </c>
       <c r="D54" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1686,31 +1708,31 @@
       </c>
       <c r="D57" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1718,15 +1740,15 @@
       </c>
       <c r="D59" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1734,15 +1756,15 @@
       </c>
       <c r="D60" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1750,15 +1772,15 @@
       </c>
       <c r="D61" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1766,15 +1788,15 @@
       </c>
       <c r="D62" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1782,15 +1804,15 @@
       </c>
       <c r="D63" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1798,335 +1820,335 @@
       </c>
       <c r="D64" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66:C97" ca="1" si="2">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D66" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D67" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>11</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D67" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D68" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="D69" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="D70" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="D71" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C72" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="D72" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="D73" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>19</v>
-      </c>
-      <c r="C74" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D74" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D75" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="D76" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="D77" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="D78" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="D79" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D80" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D81" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>17</v>
-      </c>
-      <c r="C81" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D81" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="C82:C113" ca="1" si="2">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <v>1</v>
       </c>
       <c r="D82" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C85" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2134,31 +2156,31 @@
       </c>
       <c r="D85" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C86" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C87" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2166,15 +2188,15 @@
       </c>
       <c r="D87" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C88" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2182,15 +2204,15 @@
       </c>
       <c r="D88" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C89" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2198,15 +2220,15 @@
       </c>
       <c r="D89" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C90" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2214,15 +2236,15 @@
       </c>
       <c r="D90" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C91" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2230,15 +2252,15 @@
       </c>
       <c r="D91" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C92" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2246,15 +2268,15 @@
       </c>
       <c r="D92" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C93" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2262,15 +2284,15 @@
       </c>
       <c r="D93" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C94" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2278,19 +2300,19 @@
       </c>
       <c r="D94" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
@@ -2299,10 +2321,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C96" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2310,226 +2332,226 @@
       </c>
       <c r="D96" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C98" s="1">
-        <f t="shared" ref="C98:C121" ca="1" si="3">IF(RAND() &lt; 0.7, 1, 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D98" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C99" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D99" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C100" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D100" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C101" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="D101" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C102" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D102" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C103" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D103" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D104" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
         <v>15</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C104" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D104" s="1">
-        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C105" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D105" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C106" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="D106" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C107" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D107" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C108" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D108" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C109" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D109" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C110" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D110" s="1">
@@ -2539,74 +2561,74 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C111" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D111" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C112" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D112" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C113" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D113" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C114" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="C114:C137" ca="1" si="3">IF(RAND() &lt; 0.7, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="D114" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C115" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -2614,15 +2636,15 @@
       </c>
       <c r="D115" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C116" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -2630,31 +2652,31 @@
       </c>
       <c r="D116" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C117" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C118" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -2662,15 +2684,15 @@
       </c>
       <c r="D118" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C119" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -2678,15 +2700,15 @@
       </c>
       <c r="D119" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C120" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -2694,23 +2716,279 @@
       </c>
       <c r="D120" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C121" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D121" s="1">
         <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C122" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D122" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D123" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D124" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="C125" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D125" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C126" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D126" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C127" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D127" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C128" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D128" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D129" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C130" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D130" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D131" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D132" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D133" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D134" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C135" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D135" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D136" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C137" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D137" s="1">
+        <f ca="1">_xlfn.FLOOR.MATH(SQRT(POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],2,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],2,FALSE), 2)+POWER(VLOOKUP(Table2[[#This Row],[Node_A]],Table1[],3,FALSE)-VLOOKUP(Table2[[#This Row],[Node_B]],Table1[],3,FALSE), 2)+(RAND()*9)))</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>